<commit_message>
[0034] Add strongholds, new battle bgs
</commit_message>
<xml_diff>
--- a/wip/excel/Strongholds.xlsx
+++ b/wip/excel/Strongholds.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GFF Online\gff-online\wip\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GFF Online\gff-online\wip\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD0DBA7A-9F34-4367-A8ED-C2519665858C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B03F2A-7A3B-4A27-8DFC-774609FE5A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="15700" xr2:uid="{B6169786-A97A-44B7-AF5F-15269EEF7820}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="43200" windowHeight="11235" activeTab="3" xr2:uid="{B6169786-A97A-44B7-AF5F-15269EEF7820}"/>
   </bookViews>
   <sheets>
     <sheet name="Tower" sheetId="1" r:id="rId1"/>
     <sheet name="Dungeon" sheetId="2" r:id="rId2"/>
-    <sheet name="Fortress" sheetId="3" r:id="rId3"/>
-    <sheet name="Keep" sheetId="4" r:id="rId4"/>
+    <sheet name="Keep" sheetId="4" r:id="rId3"/>
+    <sheet name="Fortress" sheetId="3" r:id="rId4"/>
     <sheet name="Castle" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -97,13 +97,13 @@
     <t>Size: ~81 rooms</t>
   </si>
   <si>
-    <t>Size: ~75 rooms</t>
-  </si>
-  <si>
     <t>Size: ~63 rooms</t>
   </si>
   <si>
     <t>Size: ~70 rooms</t>
+  </si>
+  <si>
+    <t>Size: ~83 rooms</t>
   </si>
 </sst>
 </file>
@@ -119,7 +119,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -138,6 +138,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -151,10 +157,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -470,176 +477,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D0389C4-AA68-4868-A12E-CEE12AB071F8}">
-  <dimension ref="A1:BC7"/>
+  <dimension ref="A1:BC5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AC9" sqref="AC9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.7265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="AB3" s="3"/>
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
       <c r="AE3" s="1"/>
-      <c r="AF3" s="3"/>
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
       <c r="AI3" s="1"/>
-      <c r="AJ3" s="3"/>
       <c r="AK3" s="1"/>
       <c r="AL3" s="1"/>
       <c r="AM3" s="1"/>
-      <c r="AN3" s="3"/>
       <c r="AO3" s="1"/>
       <c r="AP3" s="1"/>
       <c r="AQ3" s="1"/>
-      <c r="AR3" s="3"/>
       <c r="AS3" s="1"/>
       <c r="AT3" s="1"/>
       <c r="AU3" s="1"/>
-      <c r="AV3" s="3"/>
       <c r="AW3" s="1"/>
       <c r="AX3" s="1"/>
       <c r="AY3" s="1"/>
-      <c r="AZ3" s="3"/>
       <c r="BA3" s="1"/>
       <c r="BB3" s="1"/>
       <c r="BC3" s="1"/>
     </row>
-    <row r="4" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="AB4" s="3"/>
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
       <c r="AE4" s="1"/>
-      <c r="AF4" s="3"/>
       <c r="AG4" s="1"/>
       <c r="AH4" s="1"/>
       <c r="AI4" s="1"/>
-      <c r="AJ4" s="3"/>
       <c r="AK4" s="1"/>
       <c r="AL4" s="1"/>
       <c r="AM4" s="1"/>
-      <c r="AN4" s="3"/>
       <c r="AO4" s="1"/>
       <c r="AP4" s="1"/>
       <c r="AQ4" s="1"/>
-      <c r="AR4" s="3"/>
       <c r="AS4" s="1"/>
       <c r="AT4" s="1"/>
       <c r="AU4" s="1"/>
-      <c r="AV4" s="3"/>
       <c r="AW4" s="1"/>
       <c r="AX4" s="1"/>
       <c r="AY4" s="1"/>
-      <c r="AZ4" s="3"/>
       <c r="BA4" s="1"/>
       <c r="BB4" s="1"/>
       <c r="BC4" s="1"/>
     </row>
-    <row r="5" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB5" s="3"/>
+        <v>22</v>
+      </c>
       <c r="AC5" s="1"/>
       <c r="AD5" s="2"/>
       <c r="AE5" s="1"/>
-      <c r="AF5" s="3"/>
       <c r="AG5" s="1"/>
       <c r="AH5" s="1"/>
       <c r="AI5" s="1"/>
-      <c r="AJ5" s="3"/>
       <c r="AK5" s="1"/>
       <c r="AL5" s="1"/>
       <c r="AM5" s="1"/>
-      <c r="AN5" s="3"/>
       <c r="AO5" s="1"/>
       <c r="AP5" s="1"/>
       <c r="AQ5" s="1"/>
-      <c r="AR5" s="3"/>
       <c r="AS5" s="1"/>
       <c r="AT5" s="1"/>
       <c r="AU5" s="1"/>
-      <c r="AV5" s="3"/>
       <c r="AW5" s="1"/>
       <c r="AX5" s="1"/>
       <c r="AY5" s="1"/>
-      <c r="AZ5" s="3"/>
       <c r="BA5" s="1"/>
       <c r="BB5" s="1"/>
       <c r="BC5" s="1"/>
-    </row>
-    <row r="6" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="AB6" s="3"/>
-      <c r="AC6" s="3"/>
-      <c r="AD6" s="3"/>
-      <c r="AE6" s="3"/>
-      <c r="AF6" s="3"/>
-      <c r="AG6" s="3"/>
-      <c r="AH6" s="3"/>
-      <c r="AI6" s="3"/>
-      <c r="AJ6" s="3"/>
-      <c r="AK6" s="3"/>
-      <c r="AL6" s="3"/>
-      <c r="AM6" s="3"/>
-      <c r="AN6" s="3"/>
-      <c r="AO6" s="3"/>
-      <c r="AP6" s="3"/>
-      <c r="AQ6" s="3"/>
-      <c r="AR6" s="3"/>
-      <c r="AS6" s="3"/>
-      <c r="AT6" s="3"/>
-      <c r="AU6" s="3"/>
-      <c r="AV6" s="3"/>
-      <c r="AW6" s="3"/>
-      <c r="AX6" s="3"/>
-      <c r="AY6" s="3"/>
-      <c r="AZ6" s="3"/>
-    </row>
-    <row r="7" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="AB7" s="3"/>
-      <c r="AC7" s="3"/>
-      <c r="AD7" s="3"/>
-      <c r="AE7" s="3"/>
-      <c r="AF7" s="3"/>
-      <c r="AG7" s="3"/>
-      <c r="AH7" s="3"/>
-      <c r="AI7" s="3"/>
-      <c r="AJ7" s="3"/>
-      <c r="AK7" s="3"/>
-      <c r="AL7" s="3"/>
-      <c r="AM7" s="3"/>
-      <c r="AN7" s="3"/>
-      <c r="AO7" s="3"/>
-      <c r="AP7" s="3"/>
-      <c r="AQ7" s="3"/>
-      <c r="AR7" s="3"/>
-      <c r="AS7" s="3"/>
-      <c r="AT7" s="3"/>
-      <c r="AU7" s="3"/>
-      <c r="AV7" s="3"/>
-      <c r="AW7" s="3"/>
-      <c r="AX7" s="3"/>
-      <c r="AY7" s="3"/>
-      <c r="AZ7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -648,31 +580,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD66560-182A-4803-94B9-1266221FA975}">
-  <dimension ref="A1:AP8"/>
+  <dimension ref="A1:AP7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="AE7" sqref="AE7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.7265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="Y3" s="3"/>
-      <c r="Z3" s="3"/>
-      <c r="AA3" s="3"/>
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
@@ -680,7 +609,6 @@
       <c r="AF3" s="1"/>
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
-      <c r="AI3" s="3"/>
       <c r="AJ3" s="1"/>
       <c r="AK3" s="1"/>
       <c r="AL3" s="1"/>
@@ -689,13 +617,10 @@
       <c r="AO3" s="1"/>
       <c r="AP3" s="1"/>
     </row>
-    <row r="4" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
       <c r="AB4" s="1"/>
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
@@ -703,7 +628,6 @@
       <c r="AF4" s="1"/>
       <c r="AG4" s="1"/>
       <c r="AH4" s="1"/>
-      <c r="AI4" s="3"/>
       <c r="AJ4" s="1"/>
       <c r="AK4" s="1"/>
       <c r="AL4" s="1"/>
@@ -712,13 +636,10 @@
       <c r="AO4" s="1"/>
       <c r="AP4" s="1"/>
     </row>
-    <row r="5" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y5" s="3"/>
-      <c r="Z5" s="3"/>
-      <c r="AA5" s="3"/>
+        <v>23</v>
+      </c>
       <c r="AB5" s="1"/>
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
@@ -726,7 +647,6 @@
       <c r="AF5" s="1"/>
       <c r="AG5" s="1"/>
       <c r="AH5" s="1"/>
-      <c r="AI5" s="3"/>
       <c r="AJ5" s="1"/>
       <c r="AK5" s="1"/>
       <c r="AL5" s="1"/>
@@ -735,10 +655,7 @@
       <c r="AO5" s="1"/>
       <c r="AP5" s="1"/>
     </row>
-    <row r="6" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="Y6" s="3"/>
-      <c r="Z6" s="3"/>
-      <c r="AA6" s="3"/>
+    <row r="6" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AB6" s="1"/>
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
@@ -746,7 +663,6 @@
       <c r="AF6" s="1"/>
       <c r="AG6" s="1"/>
       <c r="AH6" s="1"/>
-      <c r="AI6" s="3"/>
       <c r="AJ6" s="1"/>
       <c r="AK6" s="1"/>
       <c r="AL6" s="1"/>
@@ -755,10 +671,7 @@
       <c r="AO6" s="1"/>
       <c r="AP6" s="1"/>
     </row>
-    <row r="7" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="Y7" s="3"/>
-      <c r="Z7" s="3"/>
-      <c r="AA7" s="3"/>
+    <row r="7" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AB7" s="1"/>
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
@@ -766,7 +679,6 @@
       <c r="AF7" s="1"/>
       <c r="AG7" s="1"/>
       <c r="AH7" s="1"/>
-      <c r="AI7" s="3"/>
       <c r="AJ7" s="1"/>
       <c r="AK7" s="1"/>
       <c r="AL7" s="1"/>
@@ -775,87 +687,189 @@
       <c r="AO7" s="1"/>
       <c r="AP7" s="1"/>
     </row>
-    <row r="8" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="Y8" s="3"/>
-      <c r="Z8" s="3"/>
-      <c r="AA8" s="3"/>
-      <c r="AB8" s="3"/>
-      <c r="AC8" s="3"/>
-      <c r="AD8" s="3"/>
-      <c r="AF8" s="3"/>
-      <c r="AG8" s="3"/>
-      <c r="AH8" s="3"/>
-      <c r="AI8" s="3"/>
-      <c r="AJ8" s="3"/>
-      <c r="AK8" s="3"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B0E48CD-7609-42FD-9BE6-3728B75A95FF}">
-  <dimension ref="A1:AF12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8D20A61-9A4B-4296-BF84-C5232729EDEE}">
+  <dimension ref="A1:AI10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="AI2" sqref="AI2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.7265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
+      <c r="AI2" s="1"/>
+    </row>
+    <row r="3" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="1"/>
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1"/>
+      <c r="AG3" s="1"/>
+      <c r="AH3" s="1"/>
+      <c r="AI3" s="1"/>
+    </row>
+    <row r="4" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="1"/>
+      <c r="AE4" s="1"/>
+      <c r="AF4" s="1"/>
+      <c r="AG4" s="1"/>
+      <c r="AH4" s="1"/>
+      <c r="AI4" s="1"/>
+    </row>
+    <row r="5" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1"/>
+      <c r="AE5" s="1"/>
+      <c r="AF5" s="1"/>
+      <c r="AG5" s="1"/>
+      <c r="AH5" s="1"/>
+      <c r="AI5" s="1"/>
+    </row>
+    <row r="6" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="1"/>
+      <c r="AE6" s="1"/>
+      <c r="AF6" s="1"/>
+      <c r="AG6" s="1"/>
+      <c r="AH6" s="1"/>
+      <c r="AI6" s="1"/>
+    </row>
+    <row r="7" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="1"/>
+      <c r="AE7" s="1"/>
+      <c r="AF7" s="1"/>
+      <c r="AG7" s="1"/>
+      <c r="AH7" s="1"/>
+      <c r="AI7" s="1"/>
+    </row>
+    <row r="8" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="1"/>
+      <c r="AE8" s="1"/>
+      <c r="AF8" s="1"/>
+      <c r="AG8" s="1"/>
+      <c r="AH8" s="1"/>
+      <c r="AI8" s="1"/>
+    </row>
+    <row r="9" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="1"/>
+      <c r="AC9" s="1"/>
+      <c r="AD9" s="1"/>
+      <c r="AE9" s="1"/>
+      <c r="AF9" s="1"/>
+      <c r="AG9" s="1"/>
+      <c r="AH9" s="1"/>
+      <c r="AI9" s="1"/>
+    </row>
+    <row r="10" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+      <c r="AC10" s="1"/>
+      <c r="AD10" s="1"/>
+      <c r="AE10" s="2"/>
+      <c r="AF10" s="1"/>
+      <c r="AG10" s="1"/>
+      <c r="AH10" s="1"/>
+      <c r="AI10" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B0E48CD-7609-42FD-9BE6-3728B75A95FF}">
+  <dimension ref="A1:AE12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z3" sqref="Z3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="3"/>
-      <c r="X3" s="3"/>
-      <c r="Y3" s="3"/>
-      <c r="Z3" s="3"/>
-      <c r="AA3" s="3"/>
-      <c r="AB3" s="3"/>
-      <c r="AC3" s="3"/>
-      <c r="AD3" s="3"/>
-      <c r="AE3" s="3"/>
-      <c r="AF3" s="3"/>
-    </row>
-    <row r="4" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
-      <c r="AA4" s="1"/>
-      <c r="AB4" s="1"/>
-      <c r="AC4" s="3"/>
-      <c r="AD4" s="3"/>
-      <c r="AE4" s="3"/>
-      <c r="AF4" s="3"/>
-    </row>
-    <row r="5" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="4"/>
+      <c r="AA4" s="4"/>
+      <c r="AB4" s="4"/>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="1"/>
+      <c r="AE4" s="1"/>
+    </row>
+    <row r="5" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
-      <c r="V5" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
@@ -863,13 +877,11 @@
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
       <c r="AC5" s="1"/>
-      <c r="AD5" s="3"/>
-      <c r="AE5" s="3"/>
-      <c r="AF5" s="3"/>
-    </row>
-    <row r="6" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
+      <c r="AD5" s="1"/>
+      <c r="AE5" s="1"/>
+    </row>
+    <row r="6" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U6" s="1"/>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
@@ -879,12 +891,10 @@
       <c r="AB6" s="1"/>
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
-      <c r="AE6" s="3"/>
-      <c r="AF6" s="3"/>
-    </row>
-    <row r="7" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="T7" s="3"/>
-      <c r="U7" s="1"/>
+      <c r="AE6" s="1"/>
+    </row>
+    <row r="7" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U7" s="4"/>
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
       <c r="X7" s="1"/>
@@ -894,12 +904,10 @@
       <c r="AB7" s="1"/>
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
-      <c r="AE7" s="1"/>
-      <c r="AF7" s="3"/>
-    </row>
-    <row r="8" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="T8" s="3"/>
-      <c r="U8" s="1"/>
+      <c r="AE7" s="4"/>
+    </row>
+    <row r="8" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U8" s="4"/>
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
@@ -909,11 +917,10 @@
       <c r="AB8" s="1"/>
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
-      <c r="AE8" s="1"/>
-    </row>
-    <row r="9" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="T9" s="3"/>
-      <c r="U9" s="1"/>
+      <c r="AE8" s="4"/>
+    </row>
+    <row r="9" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U9" s="4"/>
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
@@ -923,11 +930,10 @@
       <c r="AB9" s="1"/>
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
-      <c r="AE9" s="1"/>
-    </row>
-    <row r="10" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="T10" s="3"/>
-      <c r="U10" s="3"/>
+      <c r="AE9" s="4"/>
+    </row>
+    <row r="10" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U10" s="1"/>
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
@@ -937,163 +943,33 @@
       <c r="AB10" s="1"/>
       <c r="AC10" s="1"/>
       <c r="AD10" s="1"/>
-    </row>
-    <row r="11" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="T11" s="3"/>
-      <c r="U11" s="3"/>
-      <c r="V11" s="3"/>
+      <c r="AE10" s="1"/>
+    </row>
+    <row r="11" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
-      <c r="Z11" s="1"/>
+      <c r="Z11" s="3"/>
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
       <c r="AC11" s="1"/>
-      <c r="AD11" s="3"/>
-    </row>
-    <row r="12" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="T12" s="3"/>
-      <c r="U12" s="3"/>
-      <c r="V12" s="3"/>
-      <c r="W12" s="3"/>
-      <c r="X12" s="1"/>
-      <c r="Y12" s="1"/>
-      <c r="Z12" s="2"/>
-      <c r="AA12" s="1"/>
-      <c r="AB12" s="1"/>
-      <c r="AC12" s="3"/>
-      <c r="AD12" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8D20A61-9A4B-4296-BF84-C5232729EDEE}">
-  <dimension ref="A1:AI10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="2.7265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
-      <c r="AE2" s="1"/>
-      <c r="AF2" s="1"/>
-      <c r="AG2" s="1"/>
-      <c r="AH2" s="1"/>
-      <c r="AI2" s="1"/>
-    </row>
-    <row r="3" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA3" s="1"/>
-      <c r="AB3" s="1"/>
-      <c r="AC3" s="1"/>
-      <c r="AD3" s="1"/>
-      <c r="AE3" s="1"/>
-      <c r="AF3" s="1"/>
-      <c r="AG3" s="1"/>
-      <c r="AH3" s="1"/>
-      <c r="AI3" s="1"/>
-    </row>
-    <row r="4" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="AA4" s="1"/>
-      <c r="AB4" s="1"/>
-      <c r="AC4" s="1"/>
-      <c r="AD4" s="1"/>
-      <c r="AE4" s="1"/>
-      <c r="AF4" s="1"/>
-      <c r="AG4" s="1"/>
-      <c r="AH4" s="1"/>
-      <c r="AI4" s="1"/>
-    </row>
-    <row r="5" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="AA5" s="1"/>
-      <c r="AB5" s="1"/>
-      <c r="AC5" s="1"/>
-      <c r="AD5" s="1"/>
-      <c r="AE5" s="1"/>
-      <c r="AF5" s="1"/>
-      <c r="AG5" s="1"/>
-      <c r="AH5" s="1"/>
-      <c r="AI5" s="1"/>
-    </row>
-    <row r="6" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="AA6" s="1"/>
-      <c r="AB6" s="1"/>
-      <c r="AC6" s="1"/>
-      <c r="AD6" s="1"/>
-      <c r="AE6" s="1"/>
-      <c r="AF6" s="1"/>
-      <c r="AG6" s="1"/>
-      <c r="AH6" s="1"/>
-      <c r="AI6" s="1"/>
-    </row>
-    <row r="7" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="AA7" s="1"/>
-      <c r="AB7" s="1"/>
-      <c r="AC7" s="1"/>
-      <c r="AD7" s="1"/>
-      <c r="AE7" s="1"/>
-      <c r="AF7" s="1"/>
-      <c r="AG7" s="1"/>
-      <c r="AH7" s="1"/>
-      <c r="AI7" s="1"/>
-    </row>
-    <row r="8" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="AA8" s="1"/>
-      <c r="AB8" s="1"/>
-      <c r="AC8" s="1"/>
-      <c r="AD8" s="1"/>
-      <c r="AE8" s="1"/>
-      <c r="AF8" s="1"/>
-      <c r="AG8" s="1"/>
-      <c r="AH8" s="1"/>
-      <c r="AI8" s="1"/>
-    </row>
-    <row r="9" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="AA9" s="1"/>
-      <c r="AB9" s="1"/>
-      <c r="AC9" s="1"/>
-      <c r="AD9" s="1"/>
-      <c r="AE9" s="1"/>
-      <c r="AF9" s="1"/>
-      <c r="AG9" s="1"/>
-      <c r="AH9" s="1"/>
-      <c r="AI9" s="1"/>
-    </row>
-    <row r="10" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="AA10" s="1"/>
-      <c r="AB10" s="1"/>
-      <c r="AC10" s="1"/>
-      <c r="AD10" s="1"/>
-      <c r="AE10" s="2"/>
-      <c r="AF10" s="1"/>
-      <c r="AG10" s="1"/>
-      <c r="AH10" s="1"/>
-      <c r="AI10" s="1"/>
+      <c r="AD11" s="1"/>
+      <c r="AE11" s="1"/>
+    </row>
+    <row r="12" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="4"/>
+      <c r="Y12" s="4"/>
+      <c r="Z12" s="4"/>
+      <c r="AA12" s="4"/>
+      <c r="AB12" s="4"/>
+      <c r="AC12" s="1"/>
+      <c r="AD12" s="1"/>
+      <c r="AE12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1105,22 +981,22 @@
   <dimension ref="A1:BK11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AA22" sqref="AA22"/>
+      <selection activeCell="AK11" sqref="AK11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.7265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1137,7 +1013,7 @@
       <c r="BJ3" s="1"/>
       <c r="BK3" s="1"/>
     </row>
-    <row r="4" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1164,7 +1040,7 @@
       <c r="BJ4" s="1"/>
       <c r="BK4" s="1"/>
     </row>
-    <row r="5" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1178,7 +1054,7 @@
       <c r="AQ5" s="1"/>
       <c r="AW5" s="1"/>
     </row>
-    <row r="6" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AD6" s="1"/>
       <c r="AE6" s="1"/>
       <c r="AF6" s="1"/>
@@ -1189,7 +1065,7 @@
       <c r="AQ6" s="1"/>
       <c r="AW6" s="1"/>
     </row>
-    <row r="7" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AD7" s="1"/>
       <c r="AE7" s="1"/>
       <c r="AF7" s="1"/>
@@ -1200,7 +1076,7 @@
       <c r="AQ7" s="1"/>
       <c r="AW7" s="1"/>
     </row>
-    <row r="8" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AD8" s="1"/>
       <c r="AE8" s="1"/>
       <c r="AF8" s="1"/>
@@ -1211,7 +1087,7 @@
       <c r="AQ8" s="1"/>
       <c r="AW8" s="1"/>
     </row>
-    <row r="9" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AD9" s="1"/>
       <c r="AE9" s="1"/>
       <c r="AF9" s="1"/>
@@ -1222,7 +1098,7 @@
       <c r="AQ9" s="1"/>
       <c r="AW9" s="1"/>
     </row>
-    <row r="10" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC10" s="1"/>
       <c r="AD10" s="1"/>
       <c r="AE10" s="1"/>
@@ -1246,7 +1122,7 @@
       <c r="BJ10" s="1"/>
       <c r="BK10" s="1"/>
     </row>
-    <row r="11" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC11" s="1"/>
       <c r="AD11" s="1"/>
       <c r="AJ11" s="1"/>

</xml_diff>

<commit_message>
[0042] Add locks, prophets, prisoners
</commit_message>
<xml_diff>
--- a/wip/excel/Strongholds.xlsx
+++ b/wip/excel/Strongholds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GFF Online\gff-online\wip\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B03F2A-7A3B-4A27-8DFC-774609FE5A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C601FB-319E-418D-BB6E-AEA4798D9DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="43200" windowHeight="11235" activeTab="3" xr2:uid="{B6169786-A97A-44B7-AF5F-15269EEF7820}"/>
+    <workbookView xWindow="1900" yWindow="1900" windowWidth="21600" windowHeight="11320" activeTab="4" xr2:uid="{B6169786-A97A-44B7-AF5F-15269EEF7820}"/>
   </bookViews>
   <sheets>
     <sheet name="Tower" sheetId="1" r:id="rId1"/>
@@ -91,9 +91,6 @@
     <t>Armour: Helmet of Salvation</t>
   </si>
   <si>
-    <t>Size: ~112 rooms</t>
-  </si>
-  <si>
     <t>Size: ~81 rooms</t>
   </si>
   <si>
@@ -104,6 +101,9 @@
   </si>
   <si>
     <t>Size: ~83 rooms</t>
+  </si>
+  <si>
+    <t>Size: ~113 rooms</t>
   </si>
 </sst>
 </file>
@@ -157,12 +157,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,19 +482,19 @@
       <selection activeCell="AC9" sqref="AC9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="2.7265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -521,7 +520,7 @@
       <c r="BB3" s="1"/>
       <c r="BC3" s="1"/>
     </row>
-    <row r="4" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -547,9 +546,9 @@
       <c r="BB4" s="1"/>
       <c r="BC4" s="1"/>
     </row>
-    <row r="5" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AC5" s="1"/>
       <c r="AD5" s="2"/>
@@ -586,19 +585,19 @@
       <selection activeCell="AE7" sqref="AE7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="2.7265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -617,7 +616,7 @@
       <c r="AO3" s="1"/>
       <c r="AP3" s="1"/>
     </row>
-    <row r="4" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -636,9 +635,9 @@
       <c r="AO4" s="1"/>
       <c r="AP4" s="1"/>
     </row>
-    <row r="5" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AB5" s="1"/>
       <c r="AC5" s="1"/>
@@ -655,7 +654,7 @@
       <c r="AO5" s="1"/>
       <c r="AP5" s="1"/>
     </row>
-    <row r="6" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="AB6" s="1"/>
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
@@ -671,7 +670,7 @@
       <c r="AO6" s="1"/>
       <c r="AP6" s="1"/>
     </row>
-    <row r="7" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="AB7" s="1"/>
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
@@ -700,14 +699,14 @@
       <selection activeCell="AI2" sqref="AI2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="2.7265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -721,7 +720,7 @@
       <c r="AH2" s="1"/>
       <c r="AI2" s="1"/>
     </row>
-    <row r="3" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -735,7 +734,7 @@
       <c r="AH3" s="1"/>
       <c r="AI3" s="1"/>
     </row>
-    <row r="4" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -749,9 +748,9 @@
       <c r="AH4" s="1"/>
       <c r="AI4" s="1"/>
     </row>
-    <row r="5" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
@@ -763,7 +762,7 @@
       <c r="AH5" s="1"/>
       <c r="AI5" s="1"/>
     </row>
-    <row r="6" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
       <c r="AC6" s="1"/>
@@ -774,7 +773,7 @@
       <c r="AH6" s="1"/>
       <c r="AI6" s="1"/>
     </row>
-    <row r="7" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
       <c r="AC7" s="1"/>
@@ -785,7 +784,7 @@
       <c r="AH7" s="1"/>
       <c r="AI7" s="1"/>
     </row>
-    <row r="8" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
       <c r="AC8" s="1"/>
@@ -796,7 +795,7 @@
       <c r="AH8" s="1"/>
       <c r="AI8" s="1"/>
     </row>
-    <row r="9" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
       <c r="AC9" s="1"/>
@@ -807,7 +806,7 @@
       <c r="AH9" s="1"/>
       <c r="AI9" s="1"/>
     </row>
-    <row r="10" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
       <c r="AC10" s="1"/>
@@ -827,46 +826,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B0E48CD-7609-42FD-9BE6-3728B75A95FF}">
   <dimension ref="A1:AE12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Z3" sqref="Z3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="2.7265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>17</v>
       </c>
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
-      <c r="X4" s="4"/>
-      <c r="Y4" s="4"/>
-      <c r="Z4" s="4"/>
-      <c r="AA4" s="4"/>
-      <c r="AB4" s="4"/>
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
       <c r="AE4" s="1"/>
     </row>
-    <row r="5" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
@@ -880,7 +874,7 @@
       <c r="AD5" s="1"/>
       <c r="AE5" s="1"/>
     </row>
-    <row r="6" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
@@ -893,8 +887,7 @@
       <c r="AD6" s="1"/>
       <c r="AE6" s="1"/>
     </row>
-    <row r="7" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="U7" s="4"/>
+    <row r="7" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
       <c r="X7" s="1"/>
@@ -904,10 +897,8 @@
       <c r="AB7" s="1"/>
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
-      <c r="AE7" s="4"/>
-    </row>
-    <row r="8" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="U8" s="4"/>
+    </row>
+    <row r="8" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
@@ -917,10 +908,8 @@
       <c r="AB8" s="1"/>
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
-      <c r="AE8" s="4"/>
-    </row>
-    <row r="9" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="U9" s="4"/>
+    </row>
+    <row r="9" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
@@ -930,9 +919,8 @@
       <c r="AB9" s="1"/>
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
-      <c r="AE9" s="4"/>
-    </row>
-    <row r="10" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
@@ -945,7 +933,7 @@
       <c r="AD10" s="1"/>
       <c r="AE10" s="1"/>
     </row>
-    <row r="11" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
@@ -958,15 +946,10 @@
       <c r="AD11" s="1"/>
       <c r="AE11" s="1"/>
     </row>
-    <row r="12" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="U12" s="1"/>
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
-      <c r="X12" s="4"/>
-      <c r="Y12" s="4"/>
-      <c r="Z12" s="4"/>
-      <c r="AA12" s="4"/>
-      <c r="AB12" s="4"/>
       <c r="AC12" s="1"/>
       <c r="AD12" s="1"/>
       <c r="AE12" s="1"/>
@@ -980,23 +963,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DD050BE-8329-46AC-8A4F-6BC113C2CC92}">
   <dimension ref="A1:BK11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AK11" sqref="AK11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="2.7265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1013,7 +996,7 @@
       <c r="BJ3" s="1"/>
       <c r="BK3" s="1"/>
     </row>
-    <row r="4" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1040,9 +1023,9 @@
       <c r="BJ4" s="1"/>
       <c r="BK4" s="1"/>
     </row>
-    <row r="5" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="AD5" s="1"/>
       <c r="AE5" s="1"/>
@@ -1054,7 +1037,7 @@
       <c r="AQ5" s="1"/>
       <c r="AW5" s="1"/>
     </row>
-    <row r="6" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="AD6" s="1"/>
       <c r="AE6" s="1"/>
       <c r="AF6" s="1"/>
@@ -1065,7 +1048,7 @@
       <c r="AQ6" s="1"/>
       <c r="AW6" s="1"/>
     </row>
-    <row r="7" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="AD7" s="1"/>
       <c r="AE7" s="1"/>
       <c r="AF7" s="1"/>
@@ -1076,7 +1059,7 @@
       <c r="AQ7" s="1"/>
       <c r="AW7" s="1"/>
     </row>
-    <row r="8" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="AD8" s="1"/>
       <c r="AE8" s="1"/>
       <c r="AF8" s="1"/>
@@ -1087,7 +1070,7 @@
       <c r="AQ8" s="1"/>
       <c r="AW8" s="1"/>
     </row>
-    <row r="9" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="AD9" s="1"/>
       <c r="AE9" s="1"/>
       <c r="AF9" s="1"/>
@@ -1098,7 +1081,7 @@
       <c r="AQ9" s="1"/>
       <c r="AW9" s="1"/>
     </row>
-    <row r="10" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="AC10" s="1"/>
       <c r="AD10" s="1"/>
       <c r="AE10" s="1"/>
@@ -1122,7 +1105,7 @@
       <c r="BJ10" s="1"/>
       <c r="BK10" s="1"/>
     </row>
-    <row r="11" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="AC11" s="1"/>
       <c r="AD11" s="1"/>
       <c r="AJ11" s="1"/>

</xml_diff>